<commit_message>
excel loading in progress
</commit_message>
<xml_diff>
--- a/static/dashboard.xlsx
+++ b/static/dashboard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/givezakat/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/givezakat/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BB8BCA-3CE0-7F46-B809-A5425977290D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070CDB09-B43B-184D-9168-CB38E40D7EB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21980" windowHeight="27300" xr2:uid="{73FE6E76-872B-5644-A670-D7E108E2E90A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21980" windowHeight="16740" xr2:uid="{73FE6E76-872B-5644-A670-D7E108E2E90A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -455,7 +455,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -494,7 +494,7 @@
     </row>
     <row r="2" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>43882</v>
+        <v>43883</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
excel loading is completed
</commit_message>
<xml_diff>
--- a/static/dashboard.xlsx
+++ b/static/dashboard.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/givezakat/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/givezakat/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070CDB09-B43B-184D-9168-CB38E40D7EB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9103F25D-8970-7345-8599-BD6806739163}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="21980" windowHeight="16740" xr2:uid="{73FE6E76-872B-5644-A670-D7E108E2E90A}"/>
   </bookViews>
@@ -53,50 +53,51 @@
 ser: 3,4,5</t>
   </si>
   <si>
-    <t>type: signin
-width: 2
-height: 1
-h3.width-half: Sign up to get unlimited access to the entire content of zakatlists
-button.primary: Sign In
-button.secondary: Sign Up for Rs 300 / Month</t>
+    <t>type: subscribe
+width: 2
+height: 1
+h6: Subscribe to stay tuned to zakatlists
+input: enter your email here
+button.default: Submit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type: footer
+width: 6
+height: 1
+p.small: Eat from their fruits, and give the due alms on the day of harvest. &lt;br&gt; - Al Quran 6:141
+facebook: facebook.com/zakatlists
+twitter: twitter.com/zakatlists
+makerlog: getmakerlog.com/@punch__lines </t>
+  </si>
+  <si>
+    <t>type: blog
+width: 2
+height: 1
+ser: 41</t>
+  </si>
+  <si>
+    <t>type: blog
+width: 2
+height: 1
+ser: 35</t>
   </si>
   <si>
     <t>type: meetup
 width: 2
 height: 1
+h3: Meetup coming in
 date: 1 Mar 2020
 button.default: Speak
 button.default: Attend
 button.default: Details</t>
   </si>
   <si>
-    <t>type: subscribe
-width: 2
-height: 1
-h6: Subscribe to stay tuned to zakatlists
-input: enter your email here
-button.default: Submit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type: footer
-width: 6
-height: 1
-p.small: Eat from their fruits, and give the due alms on the day of harvest. &lt;br&gt; - Al Quran 6:141
-facebook: facebook.com/zakatlists
-twitter: twitter.com/zakatlists
-makerlog: getmakerlog.com/@punch__lines </t>
-  </si>
-  <si>
-    <t>type: blog
-width: 2
-height: 1
-ser: 41</t>
-  </si>
-  <si>
-    <t>type: blog
-width: 2
-height: 1
-ser: 35</t>
+    <t>type: signin
+width: 2
+height: 1
+h3.w-half: Sign up to get unlimited access to the entire content of zakatlists
+button.primary: Sign In
+button.secondary: Sign Up for Rs 300 / Month</t>
   </si>
 </sst>
 </file>
@@ -454,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06056B57-AC2B-FC4C-B6E5-BFBAF5A1660A}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,22 +507,22 @@
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dashboard and course updated
</commit_message>
<xml_diff>
--- a/static/dashboard.xlsx
+++ b/static/dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/givezakat/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55139675-7E7F-9E4A-92F1-2E3292741021}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D206D1D7-9C1E-9F43-A5DE-09D10B05A5AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6820" yWindow="460" windowWidth="36280" windowHeight="23780" xr2:uid="{73FE6E76-872B-5644-A670-D7E108E2E90A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
   <si>
     <t>Day</t>
   </si>
@@ -112,6 +112,12 @@
 width: 2
 height: 1
 ser: 15</t>
+  </si>
+  <si>
+    <t>type: blog
+width: 2
+height: 1
+ser: 60</t>
   </si>
 </sst>
 </file>
@@ -467,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06056B57-AC2B-FC4C-B6E5-BFBAF5A1660A}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,6 +586,37 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43895</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
featured blog by justaashir
</commit_message>
<xml_diff>
--- a/static/dashboard.xlsx
+++ b/static/dashboard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/givezakat/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/givezakat/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0154C462-A86A-084B-9FF2-B9C862389C2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9CB93C-1312-1F48-9D84-B46752780EC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{73FE6E76-872B-5644-A670-D7E108E2E90A}"/>
+    <workbookView xWindow="11860" yWindow="6600" windowWidth="28800" windowHeight="16740" xr2:uid="{73FE6E76-872B-5644-A670-D7E108E2E90A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -159,14 +159,6 @@
 ser: 66</t>
   </si>
   <si>
-    <t>type: video
-width: 2
-height: 1
-h3: Featured Video
-p: May be I am wrong. But Quran is not wrong guys. I found it literally amazing. Listen to this video by Omar Sulaiman. It will give you chills. 
-button.youtube: Watch on Youtube*`https://www.youtube.com/watch?v=RGypeGiH4ys&amp;t=623s`</t>
-  </si>
-  <si>
     <t>type: blog
 width: 2
 height: 1
@@ -193,6 +185,15 @@
 width: 2
 height: 1
 ser: 96</t>
+  </si>
+  <si>
+    <t>type: featured_blog
+width: 2
+height: 1
+h3: Rules of being a good desi
+p: Some rules to follow if you want to lit Pakistan brighter. We here at zakatlists are bounded by these rules. 😀
+date: 6 Apr 2020
+author: &lt;a href=https://justaashir.com target=_blank&gt;Aashir&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -551,7 +552,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -762,16 +763,16 @@
         <v>43897</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>5</v>
@@ -783,7 +784,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
dashboard uploaded with blog
</commit_message>
<xml_diff>
--- a/static/dashboard.xlsx
+++ b/static/dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/givezakat/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B0B299-A6C5-D34C-A92E-C3895DFA48D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB20D7AB-9E66-F548-800D-9074BFA4864B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{73FE6E76-872B-5644-A670-D7E108E2E90A}"/>
   </bookViews>
@@ -187,13 +187,13 @@
     <t>type: blog
 width: 2
 height: 1
-ser: 97</t>
-  </si>
-  <si>
-    <t>type: blog
-width: 2
-height: 1
 ser: 99</t>
+  </si>
+  <si>
+    <t>type: blog
+width: 2
+height: 1
+ser: 100</t>
   </si>
 </sst>
 </file>
@@ -772,7 +772,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>5</v>
@@ -784,7 +784,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
update product hunt banner
</commit_message>
<xml_diff>
--- a/static/dashboard.xlsx
+++ b/static/dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/givezakat/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F58E8F3-C7F4-CB48-8A2F-97458B487988}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF487FC0-178B-0442-93E7-151CFCDD1216}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="920" windowWidth="43640" windowHeight="20860" xr2:uid="{73FE6E76-872B-5644-A670-D7E108E2E90A}"/>
   </bookViews>
@@ -316,9 +316,9 @@
     <t>type: signin
 width: 4
 height: 1
-h3: Zakatlists is Launching on Product Hunt - Today
-p.w-m-50: I have been writing blogs for nearly 140 days this year. If these blogs or our techshek conferences have impacted your life in some way, please support me on the launch day. I will remind you on phone call or email you if you feel you will forget. 
-button.default: Set a reminder*goto("https://docs.google.com/forms/d/e/1FAIpQLScRWGicOlVW-RpquUYvHD769v45XACKZydnpTJcJVWxzHW0jg/viewform?usp=sf_link")
+h3: Zakatlists is live on Product Hunt. 
+p.w-m-50: I have been writing blogs for nearly 140 days this year. If these blogs or our techshek conferences have impacted your life in some way, please upvote. 
+button.default: UpVote*goto("https://www.producthunt.com/posts/zakat-lists")
 button.default: What is Product Hunt*goto("https://www.producthunt.com/about")
 button.default: What is Zakatlists*goto("https://www.zakatlists.com/blogpost?serialNo=136")
 button.default: Sign Up*goto("https://www.zakatlists.com/signup")

</xml_diff>

<commit_message>
photos taken for portfolio
</commit_message>
<xml_diff>
--- a/static/dashboard.xlsx
+++ b/static/dashboard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/givezakat/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40319369-D901-614B-B956-D4DB715DBF53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622C0EAD-6A02-8642-A99D-8FBF52941A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{73FE6E76-872B-5644-A670-D7E108E2E90A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" xr2:uid="{73FE6E76-872B-5644-A670-D7E108E2E90A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -301,32 +301,32 @@
 svg: /icons/stars.svg</t>
   </si>
   <si>
+    <t>type: blog
+width: 2
+height: 1
+ser: 177</t>
+  </si>
+  <si>
+    <t>type: blog
+width: 2
+height: 1
+ser: 178</t>
+  </si>
+  <si>
+    <t>type: blog
+width: 2
+height: 1
+ser: 175</t>
+  </si>
+  <si>
     <t>type: meetup
 width: 2
 height: 1
 h3: Meetup coming in
-date: 2020,6,5,10,30,0,0
+date: 2023,2,2,10,30,0,0
 button.default: Speak*goto("https://forms.gle/dyydXFRSsKzeH4hZ6")
 button.default: Attend*goto("https://youtu.be/vscn-HP932E")
 button.default: Details*goto("https://www.meetup.com/techshek/events/270179438/")</t>
-  </si>
-  <si>
-    <t>type: blog
-width: 2
-height: 1
-ser: 177</t>
-  </si>
-  <si>
-    <t>type: blog
-width: 2
-height: 1
-ser: 178</t>
-  </si>
-  <si>
-    <t>type: blog
-width: 2
-height: 1
-ser: 179</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -674,7 +674,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -685,7 +685,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1010,25 +1010,25 @@
         <v>43981</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>4</v>

</xml_diff>